<commit_message>
final commit; tidied up R + added comments
</commit_message>
<xml_diff>
--- a/IXIS-analysis-scripts/analysis_results.xlsx
+++ b/IXIS-analysis-scripts/analysis_results.xlsx
@@ -13,12 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">dim_deviceCategory</t>
   </si>
   <si>
-    <t xml:space="preserve">month_number</t>
+    <t xml:space="preserve">year_after_2000</t>
   </si>
   <si>
     <t xml:space="preserve">sessions</t>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">tablet</t>
   </si>
   <si>
+    <t xml:space="preserve">metric</t>
+  </si>
+  <si>
     <t xml:space="preserve">5/13</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t xml:space="preserve">relative_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addsToCart</t>
   </si>
 </sst>
 </file>
@@ -1150,74 +1156,92 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>1164639</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>1388834</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>224195</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>1.19250171083057</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>28389</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>34538</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>6149</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>1.21659797809011</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>51629</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>61891</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>10262</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>1.19876426039629</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.0243757937008807</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>0.0248683427969073</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>0.000492549096026633</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>1.02020648443578</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="n">
         <v>136720</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>107970</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>-28750</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.789716208308953</v>
       </c>
     </row>

</xml_diff>